<commit_message>
add clean world data
</commit_message>
<xml_diff>
--- a/population_prep/world_pops_modified.xlsx
+++ b/population_prep/world_pops_modified.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17033\Desktop\shiny_covid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17033\Desktop\shiny_covid\COVID-shiny-tracker\population_prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5730594-1E32-4BB6-8E80-4CFC7E47B4EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B1F1CE-D633-41F6-B023-64C0BE951635}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{CA823E61-C46C-49C2-9279-031194C930BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CA823E61-C46C-49C2-9279-031194C930BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,9 +293,6 @@
     <t>Malaysia</t>
   </si>
   <si>
-    <t>Myanmar</t>
-  </si>
-  <si>
     <t>Philippines</t>
   </si>
   <si>
@@ -747,6 +744,9 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>Burma</t>
   </si>
 </sst>
 </file>
@@ -1115,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4BF7B5-E33E-4D57-A637-FE158C7CCC18}">
   <dimension ref="A1:C236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,13 +1128,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
         <v>190</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>191</v>
-      </c>
-      <c r="C1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1211,13 +1211,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B11" s="2">
         <v>272.81299999999999</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1230,13 +1230,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B13" s="2">
         <v>895.30799999999999</v>
       </c>
       <c r="C13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>11193.728999999999</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B19" s="2">
         <v>59734.213000000003</v>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="26" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B26" s="2">
         <v>5518.0919999999996</v>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="27" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B27" s="2">
         <v>89561.403999999995</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B39" s="2">
         <v>26378.275000000001</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="73" spans="1:2" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B73" s="2">
         <v>5101.4160000000002</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B74" s="2">
         <v>17500.656999999999</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B87" s="2">
         <v>83992.952999999994</v>
@@ -1882,7 +1882,7 @@
         <v>7496.9880000000003</v>
       </c>
       <c r="C93" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1893,12 +1893,12 @@
         <v>649.34199999999998</v>
       </c>
       <c r="C94" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B95" s="2">
         <v>23816.775000000001</v>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B96" s="2">
         <v>25778.814999999999</v>
@@ -1930,7 +1930,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B99" s="2">
         <v>51269.182999999997</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B100" s="2">
         <v>437.483</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B103" s="2">
         <v>7275.5559999999996</v>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="B105" s="2">
         <v>54409.794000000002</v>
@@ -1986,7 +1986,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B106" s="2">
         <v>109581.08500000001</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B107" s="2">
         <v>5850.3429999999998</v>
@@ -2002,7 +2002,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B108" s="2">
         <v>69799.978000000003</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B109" s="2">
         <v>1318.442</v>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B110" s="2">
         <v>97338.582999999999</v>
@@ -2026,18 +2026,18 @@
     </row>
     <row r="111" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B111" s="2">
         <v>15.002000000000001</v>
       </c>
       <c r="C111" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B112" s="2">
         <v>97.927999999999997</v>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B113" s="2">
         <v>106.76600000000001</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B114" s="2">
         <v>393.24799999999999</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B115" s="2">
         <v>287.37099999999998</v>
@@ -2069,40 +2069,40 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B116" s="2">
         <v>26.221</v>
       </c>
       <c r="C116" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B117" s="2">
         <v>30.236999999999998</v>
       </c>
       <c r="C117" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B118" s="2">
         <v>65.72</v>
       </c>
       <c r="C118" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B119" s="2">
         <v>11326.616</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B120" s="2">
         <v>164.1</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B121" s="2">
         <v>71.991</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="122" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B122" s="2">
         <v>10847.904</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B123" s="2">
         <v>112.51900000000001</v>
@@ -2142,18 +2142,18 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B124" s="2">
         <v>400.12700000000001</v>
       </c>
       <c r="C124" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B125" s="2">
         <v>11402.532999999999</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B126" s="2">
         <v>2961.1610000000001</v>
@@ -2169,29 +2169,29 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B127" s="2">
         <v>375.26499999999999</v>
       </c>
       <c r="C127" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B128" s="2">
         <v>4.9989999999999997</v>
       </c>
       <c r="C128" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B129" s="2">
         <v>2860.84</v>
@@ -2199,18 +2199,18 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B130" s="2">
         <v>9.8849999999999998</v>
       </c>
       <c r="C130" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B131" s="2">
         <v>53.192</v>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B132" s="2">
         <v>183.62899999999999</v>
@@ -2226,18 +2226,18 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B133" s="2">
         <v>38.658999999999999</v>
       </c>
       <c r="C133" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B134" s="2">
         <v>110.947</v>
@@ -2245,18 +2245,18 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B135" s="2">
         <v>42.881999999999998</v>
       </c>
       <c r="C135" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B136" s="2">
         <v>1399.491</v>
@@ -2264,18 +2264,18 @@
     </row>
     <row r="137" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B137" s="2">
         <v>38.718000000000004</v>
       </c>
       <c r="C137" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B138" s="2">
         <v>104.423</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B139" s="2">
         <v>397.62099999999998</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B140" s="2">
         <v>5094.1139999999996</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B141" s="2">
         <v>6486.201</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B142" s="2">
         <v>17915.566999999999</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B143" s="2">
         <v>9904.6080000000002</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B144" s="2">
         <v>128932.753</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B145" s="2">
         <v>6624.5540000000001</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B146" s="2">
         <v>4314.768</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B147" s="2">
         <v>45195.777000000002</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B148" s="2">
         <v>11673.029</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B149" s="2">
         <v>212559.40900000001</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B150" s="2">
         <v>19116.208999999999</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B151" s="2">
         <v>50882.883999999998</v>
@@ -2387,7 +2387,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B152" s="2">
         <v>17643.060000000001</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="153" spans="1:3" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B153" s="2">
         <v>3.4830000000000001</v>
@@ -2403,18 +2403,18 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B154" s="2">
         <v>298.68200000000002</v>
       </c>
       <c r="C154" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B155" s="2">
         <v>786.55899999999997</v>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B156" s="2">
         <v>7132.53</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B157" s="2">
         <v>32971.845999999998</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B158" s="2">
         <v>586.63400000000001</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B159" s="2">
         <v>3473.7269999999999</v>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B160" s="2">
         <v>28435.942999999999</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B161" s="2">
         <v>25499.881000000001</v>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B162" s="2">
         <v>4822.2330000000002</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B163" s="2">
         <v>896.44399999999996</v>
@@ -2486,18 +2486,18 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B164" s="2">
         <v>285.49099999999999</v>
       </c>
       <c r="C164" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B165" s="2">
         <v>8947.027</v>
@@ -2505,7 +2505,7 @@
     </row>
     <row r="166" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B166" s="2">
         <v>686.87800000000004</v>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B167" s="2">
         <v>307.14999999999998</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B168" s="2">
         <v>168.78299999999999</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B169" s="2">
         <v>119.446</v>
@@ -2537,7 +2537,7 @@
     </row>
     <row r="170" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B170" s="2">
         <v>59.194000000000003</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="171" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B171" s="2">
         <v>115.021</v>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B172" s="2">
         <v>10.834</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="173" spans="1:3" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B173" s="2">
         <v>57.557000000000002</v>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B174" s="2">
         <v>18.091999999999999</v>
@@ -2577,7 +2577,7 @@
     </row>
     <row r="175" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B175" s="2">
         <v>55.197000000000003</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B176" s="2">
         <v>17.564</v>
@@ -2593,18 +2593,18 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B177" s="2">
         <v>280.904</v>
       </c>
       <c r="C177" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B178" s="2">
         <v>1.6180000000000001</v>
@@ -2612,7 +2612,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B179" s="2">
         <v>198.41</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B180" s="2">
         <v>1.35</v>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B181" s="2">
         <v>105.697</v>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B182" s="2">
         <v>11.792</v>
@@ -2644,18 +2644,18 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183" s="2">
         <v>11.246</v>
       </c>
       <c r="C183" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B184" s="2">
         <v>9449.3209999999999</v>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B185" s="2">
         <v>6948.4449999999997</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B186" s="2">
         <v>10708.982</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B187" s="2">
         <v>9660.35</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B188" s="2">
         <v>37846.605000000003</v>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B189" s="2">
         <v>4033.9630000000002</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B190" s="2">
         <v>19237.682000000001</v>
@@ -2711,7 +2711,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B191" s="2">
         <v>145934.46</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B192" s="2">
         <v>5459.643</v>
@@ -2727,7 +2727,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B193" s="2">
         <v>43733.758999999998</v>
@@ -2735,18 +2735,18 @@
     </row>
     <row r="194" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B194" s="2">
         <v>173.85900000000001</v>
       </c>
       <c r="C194" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B195" s="2">
         <v>5792.2030000000004</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B196" s="2">
         <v>1326.539</v>
@@ -2762,18 +2762,18 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B197" s="2">
         <v>48.865000000000002</v>
       </c>
       <c r="C197" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B198" s="2">
         <v>5540.7179999999998</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B199" s="2">
         <v>341.25</v>
@@ -2789,7 +2789,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B200" s="2">
         <v>4937.7960000000003</v>
@@ -2797,18 +2797,18 @@
     </row>
     <row r="201" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B201" s="2">
         <v>85.031999999999996</v>
       </c>
       <c r="C201" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B202" s="2">
         <v>1886.202</v>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B203" s="2">
         <v>2722.2910000000002</v>
@@ -2824,7 +2824,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B204" s="2">
         <v>5421.2420000000002</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B205" s="2">
         <v>10099.27</v>
@@ -2840,7 +2840,7 @@
     </row>
     <row r="206" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B206" s="2">
         <v>67886.004000000001</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B207" s="2">
         <v>2877.8</v>
@@ -2856,7 +2856,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B208" s="2">
         <v>77.265000000000001</v>
@@ -2864,7 +2864,7 @@
     </row>
     <row r="209" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B209" s="2">
         <v>3280.8150000000001</v>
@@ -2872,7 +2872,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B210" s="2">
         <v>4105.268</v>
@@ -2880,18 +2880,18 @@
     </row>
     <row r="211" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B211" s="2">
         <v>33.691000000000003</v>
       </c>
       <c r="C211" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B212" s="2">
         <v>10423.056</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B213" s="2">
         <v>0.80900000000000005</v>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B214" s="2">
         <v>60461.828000000001</v>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B215" s="2">
         <v>441.53899999999999</v>
@@ -2923,7 +2923,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B216" s="2">
         <v>628.06200000000001</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="217" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B217" s="2">
         <v>2083.38</v>
@@ -2939,7 +2939,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B218" s="2">
         <v>10196.707</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B219" s="2">
         <v>33.938000000000002</v>
@@ -2955,7 +2955,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B220" s="2">
         <v>8737.3700000000008</v>
@@ -2963,7 +2963,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B221" s="2">
         <v>2078.9319999999998</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B222" s="2">
         <v>46754.783000000003</v>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B223" s="2">
         <v>9006.4</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B224" s="2">
         <v>11589.616</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B225" s="2">
         <v>65273.512000000002</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B226" s="2">
         <v>83783.945000000007</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B227" s="2">
         <v>38.137</v>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B228" s="2">
         <v>625.976</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B229" s="2">
         <v>39.244</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B230" s="2">
         <v>17134.873</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B231" s="2">
         <v>8654.6180000000004</v>
@@ -3051,18 +3051,18 @@
     </row>
     <row r="232" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B232" s="2">
         <v>62.273000000000003</v>
       </c>
       <c r="C232" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B233" s="2">
         <v>37742.156999999999</v>
@@ -3070,29 +3070,29 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B234" s="2">
         <v>56.771999999999998</v>
       </c>
       <c r="C234" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B235" s="2">
         <v>5.7949999999999999</v>
       </c>
       <c r="C235" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B236" s="2">
         <v>331002.647</v>

</xml_diff>